<commit_message>
Add first pie chart
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/lab1_180348.xlsx
+++ b/bin/Debug/net6.0/lab1_180348.xlsx
@@ -158,6 +158,154 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1080" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Procent rozszerzeń ilościowo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="20"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Statystyki!D1:D6</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Statystyki!E1:E6</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>
+</c:separator>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr anchorCtr="1" anchor="ctr" wrap="square" vert="horz" vertOverflow="ellipsis" spcFirstLastPara="1" rot="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="PieChart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:D16"/>
@@ -361,7 +509,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -371,53 +519,168 @@
       <c r="A1" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="0">
+        <v>37731</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="0">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0">
+        <v>40131</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
+        <v>7500</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="0">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0">
+        <v>8673</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="0">
+        <v>2855</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0">
+        <v>2855</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="0">
+        <v>2400</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0">
+        <v>1300</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1300</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0">
+        <v>169</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0">
+        <v>996</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0">
+        <v>150</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0">
+        <v>169</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0">
+        <v>150</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0">
+        <v>104</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>